<commit_message>
Bugfixes - todo: add custom functions
</commit_message>
<xml_diff>
--- a/app/config/tables/TEST/forms/TEST/TEST.xlsx
+++ b/app/config/tables/TEST/forms/TEST/TEST.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9F5A50-2D6D-4ADB-A04F-F520A2D8C117}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A00B4B-C14F-46A3-B875-10DBA2E15C9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6375" yWindow="2625" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="258">
   <si>
     <t>setting_name</t>
   </si>
@@ -779,6 +779,42 @@
   </si>
   <si>
     <t>TEST</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>lblKnown</t>
+  </si>
+  <si>
+    <t>lblUnknown</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>OVER 2 ÅR</t>
+  </si>
+  <si>
+    <t>IKKE OVER 2 ÅR</t>
+  </si>
+  <si>
+    <t>MAS DE 2 ANOS</t>
+  </si>
+  <si>
+    <t>NAO MAS DE 2 ANOS</t>
+  </si>
+  <si>
+    <t>data('ADA') &amp;&amp; data('ADA').length&gt;0 &amp;&amp; moment().diff(moment(data('ADA'), '\\D:DD,\\M:MM,\\Y:YYYY'),'years')&gt;=2</t>
   </si>
 </sst>
 </file>
@@ -1299,11 +1335,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,7 +1410,65 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>252</v>
+      </c>
+      <c r="F7" t="s">
+        <v>250</v>
+      </c>
+      <c r="G7" t="s">
+        <v>253</v>
+      </c>
+      <c r="H7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>252</v>
+      </c>
+      <c r="F9" t="s">
+        <v>251</v>
+      </c>
+      <c r="G9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3615,9 +3709,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3649,6 +3743,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
     </row>

</xml_diff>

<commit_message>
Updated TEST to show usage of adate helpers
</commit_message>
<xml_diff>
--- a/app/config/tables/TEST/forms/TEST/TEST.xlsx
+++ b/app/config/tables/TEST/forms/TEST/TEST.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A00B4B-C14F-46A3-B875-10DBA2E15C9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35843121-9256-4774-851E-2203312E1D58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="2625" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
     <sheet name="survey" sheetId="2" r:id="rId2"/>
-    <sheet name="queries" sheetId="5" r:id="rId3"/>
-    <sheet name="prompt_types" sheetId="6" r:id="rId4"/>
-    <sheet name="choices" sheetId="3" r:id="rId5"/>
-    <sheet name="model" sheetId="4" r:id="rId6"/>
+    <sheet name="calculates" sheetId="7" r:id="rId3"/>
+    <sheet name="queries" sheetId="5" r:id="rId4"/>
+    <sheet name="prompt_types" sheetId="6" r:id="rId5"/>
+    <sheet name="choices" sheetId="3" r:id="rId6"/>
+    <sheet name="model" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="266">
   <si>
     <t>setting_name</t>
   </si>
@@ -814,7 +815,31 @@
     <t>NAO MAS DE 2 ANOS</t>
   </si>
   <si>
-    <t>data('ADA') &amp;&amp; data('ADA').length&gt;0 &amp;&amp; moment().diff(moment(data('ADA'), '\\D:DD,\\M:MM,\\Y:YYYY'),'years')&gt;=2</t>
+    <t>lblbla</t>
+  </si>
+  <si>
+    <t>lblblabla</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Falsk</t>
+  </si>
+  <si>
+    <t>calculation_name</t>
+  </si>
+  <si>
+    <t>Alder {{adate.ageInYears(data('ADA'))}}</t>
+  </si>
+  <si>
+    <t>adate.ageInYears(data('ADA'))&gt;2</t>
+  </si>
+  <si>
+    <t>Ingen alder…</t>
+  </si>
+  <si>
+    <t>!adate.yearUnknown(data('ADA'))</t>
   </si>
 </sst>
 </file>
@@ -824,7 +849,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-406]General"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,6 +902,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -916,7 +948,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -943,6 +975,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{C28CC074-D3A0-48A2-81F3-B6A5CA836B7C}"/>
@@ -1335,11 +1368,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1459,7 @@
         <v>247</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1469,6 +1502,52 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>247</v>
+      </c>
+      <c r="C11" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F12" t="s">
+        <v>257</v>
+      </c>
+      <c r="G12" t="s">
+        <v>262</v>
+      </c>
+      <c r="H12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>252</v>
+      </c>
+      <c r="F14" t="s">
+        <v>258</v>
+      </c>
+      <c r="G14" t="s">
+        <v>264</v>
+      </c>
+      <c r="H14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1478,6 +1557,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA108D4-AA6D-472D-96E7-C4516EA7148E}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BBE916-BF25-4564-8A64-9F407011F034}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1553,7 +1660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328DD6A2-F953-4C0B-9442-0FB4A254DCDD}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1618,7 +1725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
   <dimension ref="A1:D140"/>
   <sheetViews>
@@ -3705,7 +3812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C120"/>
   <sheetViews>

</xml_diff>

<commit_message>
update to custompromt in TEST
</commit_message>
<xml_diff>
--- a/app/config/tables/TEST/forms/TEST/TEST.xlsx
+++ b/app/config/tables/TEST/forms/TEST/TEST.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35843121-9256-4774-851E-2203312E1D58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B553D9-E1EA-473A-93A6-B4E36CF97898}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="268">
   <si>
     <t>setting_name</t>
   </si>
@@ -840,6 +841,12 @@
   </si>
   <si>
     <t>!adate.yearUnknown(data('ADA'))</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -1368,11 +1375,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,110 +1451,122 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
-      <c r="B4" t="s">
-        <v>15</v>
+      <c r="D4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F4" t="s">
+        <v>266</v>
+      </c>
+      <c r="G4" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>247</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>252</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>250</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>253</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H8" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>252</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>251</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>254</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>247</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>252</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>257</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>262</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H13" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>252</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>258</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>264</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3816,9 +3835,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3861,6 +3880,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
     </row>
@@ -4064,7 +4094,7 @@
       <c r="B120" s="10"/>
     </row>
   </sheetData>
-  <sortState ref="F2:G93">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:G93">
     <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added adate example form
</commit_message>
<xml_diff>
--- a/app/config/tables/TEST/forms/TEST/TEST.xlsx
+++ b/app/config/tables/TEST/forms/TEST/TEST.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B553D9-E1EA-473A-93A6-B4E36CF97898}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555DE266-0589-45E4-AFC4-C93661FEF6E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="278">
   <si>
     <t>setting_name</t>
   </si>
@@ -783,9 +782,6 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>TT</t>
-  </si>
-  <si>
     <t>if</t>
   </si>
   <si>
@@ -822,31 +818,64 @@
     <t>lblblabla</t>
   </si>
   <si>
-    <t>Sand</t>
-  </si>
-  <si>
     <t>Falsk</t>
   </si>
   <si>
     <t>calculation_name</t>
   </si>
   <si>
-    <t>Alder {{adate.ageInYears(data('ADA'))}}</t>
-  </si>
-  <si>
-    <t>adate.ageInYears(data('ADA'))&gt;2</t>
-  </si>
-  <si>
     <t>Ingen alder…</t>
   </si>
   <si>
     <t>!adate.yearUnknown(data('ADA'))</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>text</t>
+    <t>display.adate.fromYear</t>
+  </si>
+  <si>
+    <t>display.adate.toYear</t>
+  </si>
+  <si>
+    <t>adate.ageInYears(data('ADA'))&gt;=2</t>
+  </si>
+  <si>
+    <t>ageInYears</t>
+  </si>
+  <si>
+    <t>ageInMonths</t>
+  </si>
+  <si>
+    <t>ageInDays</t>
+  </si>
+  <si>
+    <t>adate.diffInYears(data('ADA'), data('ADA2'))</t>
+  </si>
+  <si>
+    <t>ADA2</t>
+  </si>
+  <si>
+    <t>Testdato 2</t>
+  </si>
+  <si>
+    <t>Nammename</t>
+  </si>
+  <si>
+    <t>adate.ageInYears(data('ADA2'))</t>
+  </si>
+  <si>
+    <t>adate.ageInMonths(data('ADA2'))</t>
+  </si>
+  <si>
+    <t>adate.ageInDays(data('ADA2'))</t>
+  </si>
+  <si>
+    <t>Alder I hele år: &lt;b&gt;{{calculates.ageInYears}}&lt;/b&gt;&lt;br/&gt;I måneder: {{calculates.ageInMonths}}&lt;br/&gt;I dage: {{calculates.ageInDays}}&lt;br/&gt;( baseret på {{data.ADA}} )&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>diffInYears</t>
+  </si>
+  <si>
+    <t>Differencen var: {{calculates.diffInYears}} år.</t>
   </si>
 </sst>
 </file>
@@ -1375,28 +1404,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.5703125" customWidth="1"/>
     <col min="8" max="8" width="30" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.85546875" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>121</v>
       </c>
@@ -1427,14 +1459,20 @@
       <c r="J1" s="5" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="D3" t="s">
         <v>241</v>
@@ -1448,125 +1486,148 @@
       <c r="H3" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>1998</v>
+      </c>
+      <c r="L3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="D4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F4" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="G4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="H4" t="s">
+        <v>271</v>
+      </c>
+      <c r="K4">
+        <v>1990</v>
+      </c>
+      <c r="L4">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>251</v>
+      </c>
+      <c r="F8" t="s">
+        <v>249</v>
+      </c>
+      <c r="G8" t="s">
+        <v>252</v>
+      </c>
+      <c r="H8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>247</v>
       </c>
-      <c r="C7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>252</v>
-      </c>
-      <c r="F8" t="s">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" t="s">
         <v>250</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G10" t="s">
         <v>253</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H10" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>252</v>
-      </c>
-      <c r="F10" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>246</v>
+      </c>
+      <c r="C12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>251</v>
       </c>
-      <c r="G10" t="s">
-        <v>254</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="F13" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="G13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>251</v>
+      </c>
+      <c r="F14" t="s">
+        <v>257</v>
+      </c>
+      <c r="G14" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>247</v>
       </c>
-      <c r="C12" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>252</v>
-      </c>
-      <c r="F13" t="s">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>251</v>
+      </c>
+      <c r="F16" t="s">
         <v>257</v>
       </c>
-      <c r="G13" t="s">
-        <v>262</v>
-      </c>
-      <c r="H13" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>252</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G16" t="s">
+        <v>260</v>
+      </c>
+      <c r="H16" t="s">
         <v>258</v>
-      </c>
-      <c r="G15" t="s">
-        <v>264</v>
-      </c>
-      <c r="H15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1577,10 +1638,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA108D4-AA6D-472D-96E7-C4516EA7148E}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,10 +1652,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>276</v>
+      </c>
+      <c r="B5" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3835,9 +3928,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3866,29 +3959,18 @@
         <v>239</v>
       </c>
       <c r="C2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>269</v>
       </c>
       <c r="B3" t="s">
         <v>239</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>266</v>
-      </c>
-      <c r="B4" t="s">
-        <v>267</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4094,7 +4176,7 @@
       <c r="B120" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:G93">
+  <sortState ref="F2:G93">
     <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>